<commit_message>
unit 6 final and new datasets for problems
</commit_message>
<xml_diff>
--- a/data/film_testing.xlsx
+++ b/data/film_testing.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="63" documentId="8_{D5376C5D-3F6F-4718-A39C-5EA04CE78D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64C07C45-C0D2-4B26-A3D3-7FAB49A082BC}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="8_{D5376C5D-3F6F-4718-A39C-5EA04CE78D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C3C219A-0E69-446E-A4CD-F81485ECAF68}"/>
   <bookViews>
     <workbookView xWindow="3300" yWindow="1217" windowWidth="23949" windowHeight="15926" xr2:uid="{1D503A91-57D9-494B-A796-86E80F7058BD}"/>
   </bookViews>
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8405EA23-03DC-4854-AA40-F01477AC7C46}">
   <dimension ref="A1:E209"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -609,7 +609,7 @@
         <v>10</v>
       </c>
       <c r="E9">
-        <v>2181</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">

</xml_diff>